<commit_message>
everything works for simple OSST implementation
</commit_message>
<xml_diff>
--- a/output/aggregate_results.xlsx
+++ b/output/aggregate_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Model</t>
+          <t>Bucketizer</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -499,80 +499,6 @@
           <t>auc_mean_std</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>StandardScaler</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>SelectKBest</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CoxPH</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.661</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.473</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.291</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.485</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>StandardScaler</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SelectKBest</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Coxnet</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.665</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.473</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.288</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.485</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>